<commit_message>
Added Unity, FMOD, and Reaper projects. Started making interface sounds and implemented them in Unity project.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trito\source\repos\671-FinalProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3800386F-D9D2-46A6-8B52-9E3428BD0D8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2690EC48-71EA-4A47-95A1-0A83110B76EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17085" yWindow="270" windowWidth="24855" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
+    <workbookView xWindow="375" yWindow="600" windowWidth="27495" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -265,22 +265,35 @@
   </si>
   <si>
     <t>A medium-to-high-pitch clinking noise that players when the player deflects an enemy projectile.</t>
+  </si>
+  <si>
+    <t>Boss Theme</t>
+  </si>
+  <si>
+    <t>A medium-paced music track that plays during the boss fight. The track will change based on how much health the boss has left.</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>May change sound to use chord instead of single note. 
+Sound will require balancing when music is added.</t>
+  </si>
+  <si>
+    <t>May change sound to use chord instead of single note.
+Sound will require balancing when music is added.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once sound effects have been added, this event will lower their volume as health decreases.
+Sound will require balancing when music is added. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -323,14 +336,11 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -342,6 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CD1C86-BB31-FB43-B1BA-51A5A4089428}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -668,7 +679,7 @@
     <col min="3" max="3" width="59.5" customWidth="1"/>
     <col min="4" max="4" width="43.75" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="36.875" customWidth="1"/>
+    <col min="6" max="6" width="43.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -707,9 +718,9 @@
       <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -725,10 +736,14 @@
       <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -741,7 +756,9 @@
       <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -759,592 +776,643 @@
       <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="E8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="E16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="E17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="E18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="E20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="E21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="E22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="E23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="B24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="E24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="E25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="E26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="B27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="3"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="3"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="3"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="3"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="3"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="3"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="3"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="3"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="3"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="3"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="3"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="3"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
       <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created Player sounds and added them to the game. Started creating room-related sounds.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trito\source\repos\671-FinalProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2690EC48-71EA-4A47-95A1-0A83110B76EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C63F494-9ABF-470B-8853-B32758493FBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="600" windowWidth="27495" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
+    <workbookView xWindow="1860" yWindow="960" windowWidth="27765" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Boss Defeated</t>
   </si>
   <si>
-    <t>Player Grab Pickup</t>
-  </si>
-  <si>
     <t>Player Shoot</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Bow shooting noise</t>
   </si>
   <si>
-    <t>A medium-pitch whooshing noise that plays when the player uses their melee or charged attack.</t>
-  </si>
-  <si>
     <t>Whoosing sound</t>
   </si>
   <si>
@@ -171,18 +165,6 @@
     <t>Player Grab Key</t>
   </si>
   <si>
-    <t>A short, medium-pitch chime that plays when the player grabs a key.</t>
-  </si>
-  <si>
-    <t>A short, medium pitch chime that plays when the player grabs a health or magic pickup.</t>
-  </si>
-  <si>
-    <t>Positive-sounding chime, glass clinking/ringing noise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positive-sounding chime, key or chain clinking noise </t>
-  </si>
-  <si>
     <t>Whooshing noise, fire crackling noise</t>
   </si>
   <si>
@@ -198,12 +180,6 @@
     <t>Title Theme</t>
   </si>
   <si>
-    <t>Defeat</t>
-  </si>
-  <si>
-    <t>Victory</t>
-  </si>
-  <si>
     <t>A triumphant, medium pitch chime that plays on the menu after the player has beaten the game.</t>
   </si>
   <si>
@@ -225,33 +201,15 @@
     <t>A clay shattering noise that plays when the player breaks a jar with their sword.</t>
   </si>
   <si>
-    <t>Flowerpot breaking sound</t>
-  </si>
-  <si>
     <t xml:space="preserve">A slow-paced music track that plays on the menu once the game has ended and the corresponding chime has finished. </t>
   </si>
   <si>
     <t>Player Block Projectile</t>
   </si>
   <si>
-    <t>Room Open Door</t>
-  </si>
-  <si>
-    <t>Room Drop Key</t>
-  </si>
-  <si>
     <t>Rumble noise</t>
   </si>
   <si>
-    <t>A short, low-pitch rumbling that plays when a room is cleared and the doors open.</t>
-  </si>
-  <si>
-    <t>Positive-sounding chime, key or chain clinking noise</t>
-  </si>
-  <si>
-    <t>A short, medium pitch chime that plays when a room is cleared and a key is spawned.</t>
-  </si>
-  <si>
     <t>Human grunting noise</t>
   </si>
   <si>
@@ -276,16 +234,74 @@
     <t>Confirm</t>
   </si>
   <si>
-    <t>May change sound to use chord instead of single note. 
-Sound will require balancing when music is added.</t>
-  </si>
-  <si>
-    <t>May change sound to use chord instead of single note.
-Sound will require balancing when music is added.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Once sound effects have been added, this event will lower their volume as health decreases.
-Sound will require balancing when music is added. </t>
+    <t>Ceramic vase breaking sound</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>*1</t>
+  </si>
+  <si>
+    <t>Player Strong Attack</t>
+  </si>
+  <si>
+    <t>A low-pitch whooshing noise that plays when the player uses their charged attack.</t>
+  </si>
+  <si>
+    <t>A medium-pitch whooshing noise that plays when the player uses their melee attack.</t>
+  </si>
+  <si>
+    <t>Game Open Door</t>
+  </si>
+  <si>
+    <t>Game Press Switch</t>
+  </si>
+  <si>
+    <t>Game Drop Key</t>
+  </si>
+  <si>
+    <t>*1: Sound is finished, but will require volume balancing later.</t>
+  </si>
+  <si>
+    <t>Drinking noise</t>
+  </si>
+  <si>
+    <t>Key or chain clinking noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key or chain clinking noise </t>
+  </si>
+  <si>
+    <t>A short, medium-pitch clink that plays when the player grabs a key.</t>
+  </si>
+  <si>
+    <t>A short, medium pitch clink that plays when a room is cleared and a key is spawned.</t>
+  </si>
+  <si>
+    <t>A short, drnking sound that plays when the player grabs a health or magic potion.</t>
+  </si>
+  <si>
+    <t>Player Grab Potion</t>
+  </si>
+  <si>
+    <t>*All: Need to fix track length caused by rendering by stems.</t>
+  </si>
+  <si>
+    <t>Game Defeat</t>
+  </si>
+  <si>
+    <t>Game Victory</t>
+  </si>
+  <si>
+    <t>A low-pitch rumbling that plays when a room is cleared and the doors open.</t>
+  </si>
+  <si>
+    <t>A medium-pitch rumbling that plays when the player steps on a switch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Still needs to lower sfx and music volume as health decreases and stop playing once game has ended.
+*1 </t>
   </si>
 </sst>
 </file>
@@ -334,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -353,6 +369,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CD1C86-BB31-FB43-B1BA-51A5A4089428}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -696,7 +713,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -704,23 +721,23 @@
     </row>
     <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -728,36 +745,36 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -768,437 +785,481 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="C21" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>35</v>
+      <c r="C26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="B29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="9"/>
+      <c r="D29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="9"/>
+      <c r="F30" s="6" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
@@ -1206,7 +1267,9 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
@@ -1281,8 +1344,8 @@
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -1294,15 +1357,15 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="2"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="2"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
@@ -1378,7 +1441,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="7"/>
+      <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -1390,15 +1453,15 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
-      <c r="F54" s="3"/>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="B55" s="7"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
-      <c r="F55" s="3"/>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
@@ -1409,7 +1472,23 @@
       <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
       <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished first version of sfx. Started music. Added snapshot effect to low health sound. Started balancing and mastering.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trito\source\repos\671-FinalProject\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C63F494-9ABF-470B-8853-B32758493FBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2696BBD2-E770-49A0-9C14-82EC579A1DF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="960" windowWidth="27765" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
+    <workbookView xWindow="15750" yWindow="1665" windowWidth="28170" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
   <si>
     <t>Description</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Boss Take Damage</t>
   </si>
   <si>
-    <t>Enemy Defeated</t>
-  </si>
-  <si>
     <t>Boss Defeated</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>A medium-pitch, fire crackling noise that plays when the Boss shoots a fireball.</t>
   </si>
   <si>
-    <t>Bursting noise, crackling noise</t>
-  </si>
-  <si>
     <t>Title Theme</t>
   </si>
   <si>
@@ -192,12 +186,6 @@
     <t>A medium-pitch pinging noise that reinforces the advancement of the game.</t>
   </si>
   <si>
-    <t>A low-pitch, explosion noise that plays when the Boss is defeated by the player.</t>
-  </si>
-  <si>
-    <t>A medium-pitch, explosion noise that plays when any Enemy is defeated by the player.</t>
-  </si>
-  <si>
     <t>A clay shattering noise that plays when the player breaks a jar with their sword.</t>
   </si>
   <si>
@@ -219,9 +207,6 @@
     <t>A medium-to-low-pitch, humanoid grunt that plays when Enemy 3 is hit by the player.</t>
   </si>
   <si>
-    <t>Metal clinking noise</t>
-  </si>
-  <si>
     <t>A medium-to-high-pitch clinking noise that players when the player deflects an enemy projectile.</t>
   </si>
   <si>
@@ -240,9 +225,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>*1</t>
-  </si>
-  <si>
     <t>Player Strong Attack</t>
   </si>
   <si>
@@ -261,9 +243,6 @@
     <t>Game Drop Key</t>
   </si>
   <si>
-    <t>*1: Sound is finished, but will require volume balancing later.</t>
-  </si>
-  <si>
     <t>Drinking noise</t>
   </si>
   <si>
@@ -285,9 +264,6 @@
     <t>Player Grab Potion</t>
   </si>
   <si>
-    <t>*All: Need to fix track length caused by rendering by stems.</t>
-  </si>
-  <si>
     <t>Game Defeat</t>
   </si>
   <si>
@@ -300,8 +276,53 @@
     <t>A medium-pitch rumbling that plays when the player steps on a switch.</t>
   </si>
   <si>
-    <t xml:space="preserve">Still needs to lower sfx and music volume as health decreases and stop playing once game has ended.
-*1 </t>
+    <t>Magic Blocking Noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sound was previously finished as a shield clinking noise, but has been remade as a magic noise. 
+</t>
+  </si>
+  <si>
+    <t>A low-pitch, bull groaning noise that plays when the Boss is defeated by the player.</t>
+  </si>
+  <si>
+    <t>Bull groaning noise</t>
+  </si>
+  <si>
+    <t>Enemy 3 Defeated</t>
+  </si>
+  <si>
+    <t>A medium-to-low-pitch, humanoid groan that plays when Enemy 3 is defeated by the player.</t>
+  </si>
+  <si>
+    <t>Human groaning noise</t>
+  </si>
+  <si>
+    <t>Enemy 1 Defeated</t>
+  </si>
+  <si>
+    <t>Enemy 2 Defeated</t>
+  </si>
+  <si>
+    <t>Horse groaning noise</t>
+  </si>
+  <si>
+    <t>A medium-pitch, horse-like groaning noise that plays when Enemy 1 is defeated by the player.</t>
+  </si>
+  <si>
+    <t>A medium-pitch, deer-like groaning noise that plays when Enemy 2 is defeated by the player.</t>
+  </si>
+  <si>
+    <t>Deer groaning noise</t>
+  </si>
+  <si>
+    <t>Sound still needs to be edited in both Reaper and FMOD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May revise sound later to better fit game's audio design. </t>
+  </si>
+  <si>
+    <t>*All: Need to fix track length problem caused by rendering by stems. Finished sounds will likely require further volume balancing.</t>
   </si>
 </sst>
 </file>
@@ -684,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CD1C86-BB31-FB43-B1BA-51A5A4089428}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -713,7 +734,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -721,21 +742,23 @@
     </row>
     <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2"/>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -745,39 +768,35 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -785,87 +804,97 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -875,76 +904,70 @@
         <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -955,329 +978,331 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>91</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>71</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>19</v>
+      <c r="C23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>47</v>
+      <c r="C24" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>19</v>
+      <c r="C25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>19</v>
+        <v>46</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>19</v>
+        <v>57</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>19</v>
+      <c r="C28" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>49</v>
+      <c r="C29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="6" t="s">
+    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+      <c r="E31" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="9"/>
+      <c r="F32" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
@@ -1360,8 +1385,8 @@
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -1373,15 +1398,15 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="2"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
-      <c r="F45" s="2"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
@@ -1457,7 +1482,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="7"/>
+      <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -1469,15 +1494,15 @@
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
-      <c r="F56" s="3"/>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="B57" s="7"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
-      <c r="F57" s="3"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
@@ -1488,7 +1513,23 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
       <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished editing music. Added footstep sounds. Various fixes and changes.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trito\source\repos\671-FinalProject\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trito\source\repos\671-Final-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2696BBD2-E770-49A0-9C14-82EC579A1DF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA65C6B-C332-4B2D-ABAD-DBB1D059EB40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15750" yWindow="1665" windowWidth="28170" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
+    <workbookView xWindow="3090" yWindow="840" windowWidth="28170" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
   <si>
     <t>Description</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Interface</t>
   </si>
   <si>
-    <t>Selection Change</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>Assets Required</t>
   </si>
   <si>
-    <t>Dungeon Theme</t>
-  </si>
-  <si>
     <t>Player Attack</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Not Done</t>
-  </si>
-  <si>
     <t xml:space="preserve">A medium-paced music track that plays throughout the level. </t>
   </si>
   <si>
@@ -171,15 +162,9 @@
     <t>A medium-pitch, fire crackling noise that plays when the Boss shoots a fireball.</t>
   </si>
   <si>
-    <t>Title Theme</t>
-  </si>
-  <si>
     <t>A triumphant, medium pitch chime that plays on the menu after the player has beaten the game.</t>
   </si>
   <si>
-    <t>Menu Theme</t>
-  </si>
-  <si>
     <t>Medium-pitch verse</t>
   </si>
   <si>
@@ -189,9 +174,6 @@
     <t>A clay shattering noise that plays when the player breaks a jar with their sword.</t>
   </si>
   <si>
-    <t xml:space="preserve">A slow-paced music track that plays on the menu once the game has ended and the corresponding chime has finished. </t>
-  </si>
-  <si>
     <t>Player Block Projectile</t>
   </si>
   <si>
@@ -210,12 +192,6 @@
     <t>A medium-to-high-pitch clinking noise that players when the player deflects an enemy projectile.</t>
   </si>
   <si>
-    <t>Boss Theme</t>
-  </si>
-  <si>
-    <t>A medium-paced music track that plays during the boss fight. The track will change based on how much health the boss has left.</t>
-  </si>
-  <si>
     <t>Confirm</t>
   </si>
   <si>
@@ -240,9 +216,6 @@
     <t>Game Press Switch</t>
   </si>
   <si>
-    <t>Game Drop Key</t>
-  </si>
-  <si>
     <t>Drinking noise</t>
   </si>
   <si>
@@ -256,9 +229,6 @@
   </si>
   <si>
     <t>A short, medium pitch clink that plays when a room is cleared and a key is spawned.</t>
-  </si>
-  <si>
-    <t>A short, drnking sound that plays when the player grabs a health or magic potion.</t>
   </si>
   <si>
     <t>Player Grab Potion</t>
@@ -316,13 +286,55 @@
     <t>Deer groaning noise</t>
   </si>
   <si>
-    <t>Sound still needs to be edited in both Reaper and FMOD.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May revise sound later to better fit game's audio design. </t>
-  </si>
-  <si>
-    <t>*All: Need to fix track length problem caused by rendering by stems. Finished sounds will likely require further volume balancing.</t>
+    <t>A medium-paced music track that plays during the boss fight. The music changes wonce the boss has reached half health.</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A slow-paced music track that plays on the menu once the game has been lost and the corresponding chime has finished. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A slow-paced music track that plays on the menu once the game has been won and the corresponding chime has finished. </t>
+  </si>
+  <si>
+    <t>Victory Music</t>
+  </si>
+  <si>
+    <t>Defeat Music</t>
+  </si>
+  <si>
+    <t>Dungeon Music</t>
+  </si>
+  <si>
+    <t>Title Music</t>
+  </si>
+  <si>
+    <t>Boss Music</t>
+  </si>
+  <si>
+    <t>Footsteps</t>
+  </si>
+  <si>
+    <t>Medium pitch footsteps that play when the player is walking and are randomized.</t>
+  </si>
+  <si>
+    <t>A set of footsteps that plays when the player walks through a door.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sound was previously finished as an electronic pinging noise, but has been remade as a wooden clicking noise. </t>
+  </si>
+  <si>
+    <t>Player Footsteps</t>
+  </si>
+  <si>
+    <t>Game Enter Door</t>
+  </si>
+  <si>
+    <t>Game Spawn Key</t>
+  </si>
+  <si>
+    <t>A short, drinking sound that plays when the player grabs a health or magic potion.</t>
   </si>
 </sst>
 </file>
@@ -705,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CD1C86-BB31-FB43-B1BA-51A5A4089428}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -722,7 +734,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -731,602 +743,622 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>96</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>96</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>97</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>39</v>
+      <c r="C10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>84</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="8"/>
+        <v>57</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="2"/>
+      <c r="E19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>65</v>
+        <v>95</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>65</v>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>95</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>31</v>
+        <v>5</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>65</v>
+        <v>5</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>45</v>
+        <v>83</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>47</v>
+        <v>5</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>65</v>
+        <v>42</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>65</v>
+        <v>79</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="9"/>
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
+      <c r="A35" s="6"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="9"/>
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
@@ -1401,8 +1433,8 @@
       <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -1414,7 +1446,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
-      <c r="F46" s="2"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
@@ -1422,15 +1454,15 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
-      <c r="F47" s="2"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
-      <c r="F48" s="2"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
@@ -1498,7 +1530,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="B57" s="7"/>
+      <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
@@ -1510,7 +1542,7 @@
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
-      <c r="F58" s="3"/>
+      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
@@ -1518,18 +1550,42 @@
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
-      <c r="F59" s="3"/>
+      <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
+      <c r="B60" s="7"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
-      <c r="F60" s="3"/>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
       <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final fixes, balancing, and mastering.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trito\source\repos\671-Final-Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA65C6B-C332-4B2D-ABAD-DBB1D059EB40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC90FAF-8DAE-48EA-8065-D48BC228AD29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="840" windowWidth="28170" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
+    <workbookView xWindow="2265" yWindow="570" windowWidth="26805" windowHeight="17175" xr2:uid="{FFB331F4-50A9-9D4A-A2CA-6B9D4BC1DD9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="104">
   <si>
     <t>Description</t>
   </si>
@@ -81,24 +81,9 @@
     <t>A slow-paced music track that plays on the title screen.</t>
   </si>
   <si>
-    <t>Low-pitch part of intro, medium-pitch part of intro, low-pitch verse, medium-pitch chorus</t>
-  </si>
-  <si>
-    <t>Low-pitch verse, medium-pitch chorus</t>
-  </si>
-  <si>
-    <t>Heartbeat or similar double beep sound</t>
-  </si>
-  <si>
-    <t>A medium-pitch pinging noise that reinforces the change of a selected menu item.</t>
-  </si>
-  <si>
     <t>Player Break Jar</t>
   </si>
   <si>
-    <t xml:space="preserve"> A low-pitch beeping that plays when the player has one bubble or less of health remaining</t>
-  </si>
-  <si>
     <t>Enemy 2 Take Damage</t>
   </si>
   <si>
@@ -138,18 +123,6 @@
     <t>Whoosing sound</t>
   </si>
   <si>
-    <t>Medium-pitch pinging or beeping noise</t>
-  </si>
-  <si>
-    <t>Triumphant-sounding chime</t>
-  </si>
-  <si>
-    <t>Defeated-sounding chime</t>
-  </si>
-  <si>
-    <t>A defeated, medium pitch chime that plays on the menu after the player has been defeated.</t>
-  </si>
-  <si>
     <t>Player Grab Key</t>
   </si>
   <si>
@@ -162,15 +135,6 @@
     <t>A medium-pitch, fire crackling noise that plays when the Boss shoots a fireball.</t>
   </si>
   <si>
-    <t>A triumphant, medium pitch chime that plays on the menu after the player has beaten the game.</t>
-  </si>
-  <si>
-    <t>Medium-pitch verse</t>
-  </si>
-  <si>
-    <t>A medium-pitch pinging noise that reinforces the advancement of the game.</t>
-  </si>
-  <si>
     <t>A clay shattering noise that plays when the player breaks a jar with their sword.</t>
   </si>
   <si>
@@ -249,92 +213,131 @@
     <t>Magic Blocking Noise</t>
   </si>
   <si>
-    <t xml:space="preserve">Sound was previously finished as a shield clinking noise, but has been remade as a magic noise. 
+    <t>A low-pitch, bull groaning noise that plays when the Boss is defeated by the player.</t>
+  </si>
+  <si>
+    <t>Bull groaning noise</t>
+  </si>
+  <si>
+    <t>Enemy 3 Defeated</t>
+  </si>
+  <si>
+    <t>A medium-to-low-pitch, humanoid groan that plays when Enemy 3 is defeated by the player.</t>
+  </si>
+  <si>
+    <t>Human groaning noise</t>
+  </si>
+  <si>
+    <t>Enemy 1 Defeated</t>
+  </si>
+  <si>
+    <t>Enemy 2 Defeated</t>
+  </si>
+  <si>
+    <t>Horse groaning noise</t>
+  </si>
+  <si>
+    <t>A medium-pitch, horse-like groaning noise that plays when Enemy 1 is defeated by the player.</t>
+  </si>
+  <si>
+    <t>A medium-pitch, deer-like groaning noise that plays when Enemy 2 is defeated by the player.</t>
+  </si>
+  <si>
+    <t>Deer groaning noise</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Victory Music</t>
+  </si>
+  <si>
+    <t>Defeat Music</t>
+  </si>
+  <si>
+    <t>Dungeon Music</t>
+  </si>
+  <si>
+    <t>Title Music</t>
+  </si>
+  <si>
+    <t>Boss Music</t>
+  </si>
+  <si>
+    <t>Footsteps</t>
+  </si>
+  <si>
+    <t>Medium pitch footsteps that play when the player is walking and are randomized.</t>
+  </si>
+  <si>
+    <t>A set of footsteps that plays when the player walks through a door.</t>
+  </si>
+  <si>
+    <t>Player Footsteps</t>
+  </si>
+  <si>
+    <t>Game Enter Door</t>
+  </si>
+  <si>
+    <t>Game Spawn Key</t>
+  </si>
+  <si>
+    <t>A short, drinking sound that plays when the player grabs a health or magic potion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sound was previously made as a shield clinking noise, but has been remade as a magic noise. 
 </t>
   </si>
   <si>
-    <t>A low-pitch, bull groaning noise that plays when the Boss is defeated by the player.</t>
-  </si>
-  <si>
-    <t>Bull groaning noise</t>
-  </si>
-  <si>
-    <t>Enemy 3 Defeated</t>
-  </si>
-  <si>
-    <t>A medium-to-low-pitch, humanoid groan that plays when Enemy 3 is defeated by the player.</t>
-  </si>
-  <si>
-    <t>Human groaning noise</t>
-  </si>
-  <si>
-    <t>Enemy 1 Defeated</t>
-  </si>
-  <si>
-    <t>Enemy 2 Defeated</t>
-  </si>
-  <si>
-    <t>Horse groaning noise</t>
-  </si>
-  <si>
-    <t>A medium-pitch, horse-like groaning noise that plays when Enemy 1 is defeated by the player.</t>
-  </si>
-  <si>
-    <t>A medium-pitch, deer-like groaning noise that plays when Enemy 2 is defeated by the player.</t>
-  </si>
-  <si>
-    <t>Deer groaning noise</t>
-  </si>
-  <si>
-    <t>A medium-paced music track that plays during the boss fight. The music changes wonce the boss has reached half health.</t>
-  </si>
-  <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A slow-paced music track that plays on the menu once the game has been lost and the corresponding chime has finished. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A slow-paced music track that plays on the menu once the game has been won and the corresponding chime has finished. </t>
-  </si>
-  <si>
-    <t>Victory Music</t>
-  </si>
-  <si>
-    <t>Defeat Music</t>
-  </si>
-  <si>
-    <t>Dungeon Music</t>
-  </si>
-  <si>
-    <t>Title Music</t>
-  </si>
-  <si>
-    <t>Boss Music</t>
-  </si>
-  <si>
-    <t>Footsteps</t>
-  </si>
-  <si>
-    <t>Medium pitch footsteps that play when the player is walking and are randomized.</t>
-  </si>
-  <si>
-    <t>A set of footsteps that plays when the player walks through a door.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sound was previously finished as an electronic pinging noise, but has been remade as a wooden clicking noise. </t>
-  </si>
-  <si>
-    <t>Player Footsteps</t>
-  </si>
-  <si>
-    <t>Game Enter Door</t>
-  </si>
-  <si>
-    <t>Game Spawn Key</t>
-  </si>
-  <si>
-    <t>A short, drinking sound that plays when the player grabs a health or magic potion.</t>
+    <t xml:space="preserve">Sound was previously made as an electronic pinging noise, but has been remade as a wooden clicking noise. </t>
+  </si>
+  <si>
+    <t>A medium-paced music track that plays during the boss fight. The music changes once the boss has reached half health.</t>
+  </si>
+  <si>
+    <t>Medium-pitch clicking noise</t>
+  </si>
+  <si>
+    <t>A medium-pitch clicking noise that reinforces the change of a selected menu item.</t>
+  </si>
+  <si>
+    <t>A clikcing noise with increasing pitch that reinforces the advancement of the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A slow-paced music track that plays on the menu once the game has been lost and the defeat chime has finished. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A slow-paced music track that plays on the menu once the game has been won and the victory chime has finished. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A low-pitch heartbeat that plays when the player has one bubble or less of health remaining</t>
+  </si>
+  <si>
+    <t>Heartbeat sound</t>
+  </si>
+  <si>
+    <t>Slow, adventurous music track</t>
+  </si>
+  <si>
+    <t>Dramatic orchestral music track</t>
+  </si>
+  <si>
+    <t>Underground-themed music track</t>
+  </si>
+  <si>
+    <t>Slow, ambient music track</t>
+  </si>
+  <si>
+    <t>Defeated-sounding jingle</t>
+  </si>
+  <si>
+    <t>Triumphant-sounding jingle</t>
+  </si>
+  <si>
+    <t>A triumphant jingle that plays on the menu after the player has beaten the game.</t>
+  </si>
+  <si>
+    <t>A defeated jingle that plays on the menu after the player has been defeated.</t>
   </si>
 </sst>
 </file>
@@ -720,7 +723,7 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -752,9 +755,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -763,56 +766,56 @@
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -821,100 +824,100 @@
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F10" s="8"/>
     </row>
@@ -926,13 +929,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F11" s="8"/>
     </row>
@@ -944,31 +947,31 @@
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F13" s="8"/>
     </row>
@@ -980,34 +983,34 @@
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1018,283 +1021,283 @@
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -1306,13 +1309,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -1324,13 +1327,13 @@
         <v>5</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -1342,13 +1345,13 @@
         <v>5</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F34" s="2"/>
     </row>

</xml_diff>